<commit_message>
fix validation and upload
</commit_message>
<xml_diff>
--- a/files/buses.xlsx
+++ b/files/buses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12360"/>
+    <workbookView windowWidth="28800" windowHeight="11915"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -27,48 +27,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
-    <t>14F</t>
+    <t>Model-2</t>
   </si>
   <si>
-    <t>549648</t>
+    <t>Model-3</t>
   </si>
   <si>
-    <t>15F</t>
+    <t>Model-4</t>
   </si>
   <si>
-    <t>062831</t>
+    <t>Model-6</t>
   </si>
   <si>
-    <t>16F</t>
-  </si>
-  <si>
-    <t>776010</t>
-  </si>
-  <si>
-    <t>17F</t>
-  </si>
-  <si>
-    <t>055170</t>
-  </si>
-  <si>
-    <t>18F</t>
-  </si>
-  <si>
-    <t>406573</t>
-  </si>
-  <si>
-    <t>19F</t>
-  </si>
-  <si>
-    <t>000356</t>
-  </si>
-  <si>
-    <t>20F</t>
-  </si>
-  <si>
-    <t>515527</t>
+    <t>Model-7</t>
   </si>
 </sst>
 </file>
@@ -684,17 +657,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1233,7 +1197,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1242,77 +1206,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>156</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C1">
         <v>14567</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>14568</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="A3">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>14569</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="A4">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
       <c r="C4">
         <v>14570</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
+      <c r="A5">
+        <v>160</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
       <c r="C5">
         <v>14571</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
+      <c r="A6">
+        <v>161</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
       </c>
       <c r="C6">
         <v>14572</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
+      <c r="A7">
+        <v>162</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
       </c>
       <c r="C7">
         <v>14573</v>

</xml_diff>